<commit_message>
move class creation upper and add empty cell #164
</commit_message>
<xml_diff>
--- a/tests/header_select/result_has_header.xlsx
+++ b/tests/header_select/result_has_header.xlsx
@@ -452,16 +452,8 @@
   <sheetFormatPr baseColWidth="8" defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
     <row r="1" ht="12.8" customHeight="1" s="1">
-      <c r="A1" s="2" t="inlineStr">
-        <is>
-          <t>header1</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr">
-        <is>
-          <t>header2</t>
-        </is>
-      </c>
+      <c r="A1" s="2" t="inlineStr"/>
+      <c r="B1" s="2" t="inlineStr"/>
     </row>
     <row r="2" ht="12.8" customHeight="1" s="1">
       <c r="A2" s="2" t="n">

</xml_diff>

<commit_message>
add run and cycle run #191
</commit_message>
<xml_diff>
--- a/tests/header_select/result_has_header.xlsx
+++ b/tests/header_select/result_has_header.xlsx
@@ -478,8 +478,8 @@
       </c>
     </row>
     <row r="3" ht="12.8" customHeight="1" s="2">
-      <c r="A3" s="3" t="inlineStr"/>
-      <c r="B3" s="3" t="inlineStr"/>
+      <c r="A3" s="3" t="n"/>
+      <c r="B3" s="3" t="n"/>
     </row>
     <row r="4" ht="12.8" customHeight="1" s="2">
       <c r="A4" s="3" t="n">
@@ -501,10 +501,7 @@
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-    </row>
+    <row r="6"/>
     <row r="7" ht="12.8" customHeight="1" s="2">
       <c r="A7" s="3" t="n">
         <v>6</v>

</xml_diff>